<commit_message>
added info to the PH plan about the valve code
</commit_message>
<xml_diff>
--- a/TMA_PH_Plan.xlsx
+++ b/TMA_PH_Plan.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12780" yWindow="2720" windowWidth="32340" windowHeight="19500" tabRatio="500"/>
+    <workbookView xWindow="12780" yWindow="2720" windowWidth="32340" windowHeight="19500" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="8-29-17" sheetId="3" r:id="rId1"/>
     <sheet name="8-8-17" sheetId="2" r:id="rId2"/>
     <sheet name="Template" sheetId="1" r:id="rId3"/>
+    <sheet name="valveCode" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="63">
   <si>
     <t>We have 11 jars currently</t>
   </si>
@@ -194,6 +195,30 @@
   </si>
   <si>
     <t>high 6mM and high 9mM were from different stock makeup; messed up the jars and had to make new 6 and 9mM and then added enough NaOH to bring to high pH</t>
+  </si>
+  <si>
+    <t>valve</t>
+  </si>
+  <si>
+    <t>Odor</t>
+  </si>
+  <si>
+    <t>clean</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>TMA</t>
+  </si>
+  <si>
+    <t>Concentration</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>Linalool</t>
   </si>
 </sst>
 </file>
@@ -392,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -420,6 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,7 +728,7 @@
   </sheetPr>
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -1703,4 +1729,246 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="19"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>